<commit_message>
1.4.2 Change to web front end to use the Tombola RPM as the required function
</commit_message>
<xml_diff>
--- a/docs/v20 frequency to RPM.xlsx
+++ b/docs/v20 frequency to RPM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tstechnologies-my.sharepoint.com/personal/gary_twinn_net/Documents/GTFiles/PhD/Python Projects/UCL-tombola/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{9395E42E-1F15-455D-86B3-C48E73885119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C38F7914-4843-49F6-8693-BDC4FC51B495}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="8_{9395E42E-1F15-455D-86B3-C48E73885119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5ABFED5-9692-45C2-A42F-9EBA0D194F99}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="22500" windowHeight="14170" xr2:uid="{3B085894-FD2F-4122-BD83-175007415C8B}"/>
+    <workbookView xWindow="8016" yWindow="-21132" windowWidth="22500" windowHeight="14172" xr2:uid="{3B085894-FD2F-4122-BD83-175007415C8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>Hz</t>
   </si>
@@ -44,13 +44,16 @@
     <t>RPM</t>
   </si>
   <si>
-    <t xml:space="preserve">RPM = </t>
+    <t xml:space="preserve">1 RPM = </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -80,9 +83,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -198,31 +202,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70</c:v>
+                  <c:v>7000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90</c:v>
+                  <c:v>9000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1173,6 +1177,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1470,13 +1478,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21A1B5BE-A781-4679-9624-1D4BE7C4E773}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1496,111 +1507,114 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="B3">
         <v>7.92</v>
       </c>
       <c r="D3" s="1">
-        <f>B3/A3</f>
-        <v>0.79200000000000004</v>
+        <f>A3/B3</f>
+        <v>126.26262626262627</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>20</v>
+        <v>2000</v>
       </c>
       <c r="B4">
         <v>16.48</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:D11" si="0">B4/A4</f>
-        <v>0.82400000000000007</v>
+        <f t="shared" ref="D4:D11" si="0">A4/B4</f>
+        <v>121.35922330097087</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>30</v>
+        <v>3000</v>
       </c>
       <c r="B5">
         <v>25.08</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>0.83599999999999997</v>
+        <v>119.61722488038278</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>40</v>
+        <v>4000</v>
       </c>
       <c r="B6">
         <v>33.619999999999997</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>0.84049999999999991</v>
+        <v>118.97679952409281</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>50</v>
+        <v>5000</v>
       </c>
       <c r="B7">
         <v>42.15</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>0.84299999999999997</v>
+        <v>118.62396204033215</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>60</v>
+        <v>6000</v>
       </c>
       <c r="B8">
         <v>50.71</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>0.84516666666666673</v>
+        <v>118.31985801617037</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>70</v>
+        <v>7000</v>
       </c>
       <c r="B9">
         <v>59.29</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>0.84699999999999998</v>
+        <v>118.06375442739079</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>80</v>
+        <v>8000</v>
       </c>
       <c r="B10">
         <v>67.87</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>0.8483750000000001</v>
+        <v>117.87240312361868</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>90</v>
+        <v>9000</v>
       </c>
       <c r="B11">
         <v>76.48</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>0.84977777777777785</v>
-      </c>
+        <v>117.67782426778243</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
@@ -1608,10 +1622,70 @@
       </c>
       <c r="D13" s="1">
         <f>AVERAGE(D3:D11)</f>
-        <v>0.83620216049382723</v>
+        <v>119.6415195381519</v>
       </c>
       <c r="E13" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C15">
+        <v>59.9</v>
+      </c>
+      <c r="D15">
+        <f>INT(C15*$D$13)</f>
+        <v>7166</v>
+      </c>
+      <c r="E15">
+        <f>D15/$D$13</f>
+        <v>59.895595004666163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <v>60</v>
+      </c>
+      <c r="D16">
+        <f>INT(C16*$D$13)</f>
+        <v>7178</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ref="E16:E18" si="1">D16/$D$13</f>
+        <v>59.995894633476659</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <v>60.1</v>
+      </c>
+      <c r="D17">
+        <f>INT(C17*$D$13)</f>
+        <v>7190</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>60.096194262287149</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C18">
+        <v>0.1</v>
+      </c>
+      <c r="D18">
+        <f>INT(C18*$D$13)</f>
+        <v>11</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>9.1941326409618732E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>